<commit_message>
Actualización 13 de mayo de 2024- Lap HP
Se actualiza el material del repositorio del curso.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Parcial_01/Bitacora_Evaluacion_Continua_Parcial_01_NRC_124.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Parcial_01/Bitacora_Evaluacion_Continua_Parcial_01_NRC_124.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\Parcial_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB53843-2733-4FC1-800E-8C34BF6A3FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BCDB38-CC42-4911-9533-FA283D896290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="435" firstSheet="1" activeTab="1" xr2:uid="{DC130204-3B6A-4C21-A656-3052A0B0BC00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="435" activeTab="1" xr2:uid="{DC130204-3B6A-4C21-A656-3052A0B0BC00}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="1" r:id="rId1"/>
@@ -708,9 +708,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -748,7 +748,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -854,7 +854,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -996,7 +996,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6043C-6AC5-44AD-A90B-B5716D1FF3C2}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:P32"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3818,7 +3818,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:G31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3830,8 +3830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB674A3-1FC8-4AB4-B45D-CC0B6F4E4F1B}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,8 +3839,9 @@
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16" width="11.42578125" style="1"/>
+    <col min="6" max="9" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -5945,7 +5946,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>